<commit_message>
Update XLSX files - 2025-05-04 19:54:33
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4186,7 +4186,7 @@
     <t>2025-05-03 13:32:51</t>
   </si>
   <si>
-    <t>2025-05-03 13:03:08</t>
+    <t>2025-05-04 16:30:12</t>
   </si>
   <si>
     <t>2025-05-04 10:09:49</t>
@@ -4996,7 +4996,7 @@
     <t>2025-05-01 12:45:45</t>
   </si>
   <si>
-    <t>2025-05-03 06:29:43</t>
+    <t>2025-05-04 16:50:50</t>
   </si>
   <si>
     <t>2025-05-04 15:54:08</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-04 20:37:35
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -5113,7 +5113,7 @@
     <t>2025-05-01 10:02:02</t>
   </si>
   <si>
-    <t>2025-05-03 19:09:42</t>
+    <t>2025-05-04 17:19:38</t>
   </si>
   <si>
     <t>2025-05-03 03:40:29</t>
@@ -5167,7 +5167,7 @@
     <t>2025-05-03 10:21:52</t>
   </si>
   <si>
-    <t>2025-05-04 11:56:18</t>
+    <t>2025-05-04 17:11:56</t>
   </si>
   <si>
     <t>2025-05-01 08:53:38</t>
@@ -5206,7 +5206,7 @@
     <t>2025-05-03 16:10:03</t>
   </si>
   <si>
-    <t>2025-05-04 16:08:59</t>
+    <t>2025-05-04 17:18:29</t>
   </si>
   <si>
     <t>2025-04-30 19:34:18</t>
@@ -5401,7 +5401,7 @@
     <t>2025-05-02 08:45:02</t>
   </si>
   <si>
-    <t>2025-05-04 16:07:46</t>
+    <t>2025-05-04 17:15:47</t>
   </si>
   <si>
     <t>2025-04-30 13:23:24</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-04 22:11:21
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4198,7 +4198,7 @@
     <t>2025-05-04 16:30:12</t>
   </si>
   <si>
-    <t>2025-05-04 18:19:04</t>
+    <t>2025-05-04 19:10:17</t>
   </si>
   <si>
     <t>2025-05-04 16:07:45</t>
@@ -5095,7 +5095,7 @@
     <t>2025-05-01 10:53:33</t>
   </si>
   <si>
-    <t>2025-05-04 18:10:18</t>
+    <t>2025-05-04 18:37:23</t>
   </si>
   <si>
     <t>2025-05-01 12:08:06</t>
@@ -5125,7 +5125,7 @@
     <t>2025-05-01 10:02:02</t>
   </si>
   <si>
-    <t>2025-05-04 18:22:26</t>
+    <t>2025-05-04 18:24:20</t>
   </si>
   <si>
     <t>2025-05-03 03:40:29</t>
@@ -5287,7 +5287,7 @@
     <t>2025-05-04 07:30:40</t>
   </si>
   <si>
-    <t>2025-05-03 09:30:50</t>
+    <t>2025-05-04 18:23:35</t>
   </si>
   <si>
     <t>2025-05-02 16:36:22</t>
@@ -5428,7 +5428,7 @@
     <t>2025-05-01 08:17:36</t>
   </si>
   <si>
-    <t>2025-05-04 18:22:10</t>
+    <t>2025-05-04 18:26:04</t>
   </si>
   <si>
     <t>2025-05-03 04:54:41</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-04 22:59:09
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4198,7 +4198,7 @@
     <t>2025-05-04 16:30:12</t>
   </si>
   <si>
-    <t>2025-05-04 19:10:17</t>
+    <t>2025-05-04 19:13:50</t>
   </si>
   <si>
     <t>2025-05-04 16:07:45</t>
@@ -4408,7 +4408,7 @@
     <t>2025-05-02 16:47:13</t>
   </si>
   <si>
-    <t>2025-05-02 14:14:38</t>
+    <t>2025-05-04 19:23:24</t>
   </si>
   <si>
     <t>2025-05-02 14:17:48</t>
@@ -5125,7 +5125,7 @@
     <t>2025-05-01 10:02:02</t>
   </si>
   <si>
-    <t>2025-05-04 18:24:20</t>
+    <t>2025-05-04 19:36:47</t>
   </si>
   <si>
     <t>2025-05-03 03:40:29</t>
@@ -5350,7 +5350,7 @@
     <t>2025-05-03 15:54:40</t>
   </si>
   <si>
-    <t>2025-05-04 14:32:45</t>
+    <t>2025-05-04 19:15:48</t>
   </si>
   <si>
     <t>2025-05-02 16:44:34</t>
@@ -5410,7 +5410,7 @@
     <t>2025-05-02 08:50:11</t>
   </si>
   <si>
-    <t>2025-05-02 08:45:02</t>
+    <t>2025-05-04 19:17:08</t>
   </si>
   <si>
     <t>2025-05-04 17:15:47</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 00:34:59
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -5263,7 +5263,7 @@
     <t>2025-05-02 11:22:41</t>
   </si>
   <si>
-    <t>2025-05-04 15:21:18</t>
+    <t>2025-05-04 21:18:15</t>
   </si>
   <si>
     <t>2025-04-30 07:11:42</t>
@@ -5440,7 +5440,7 @@
     <t>2025-05-03 10:21:35</t>
   </si>
   <si>
-    <t>2025-05-03 14:13:49</t>
+    <t>2025-05-04 21:27:37</t>
   </si>
   <si>
     <t>2025-05-04 12:09:03</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 01:22:54
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -5164,7 +5164,7 @@
     <t>2025-05-03 07:38:09</t>
   </si>
   <si>
-    <t>2025-05-01 09:34:11</t>
+    <t>2025-05-04 21:37:08</t>
   </si>
   <si>
     <t>2025-05-01 09:04:27</t>
@@ -5440,7 +5440,7 @@
     <t>2025-05-03 10:21:35</t>
   </si>
   <si>
-    <t>2025-05-04 21:27:37</t>
+    <t>2025-05-04 21:37:26</t>
   </si>
   <si>
     <t>2025-05-04 12:09:03</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 06:58:58
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4117,7 +4117,7 @@
     <t>2025-05-04 09:11:06</t>
   </si>
   <si>
-    <t>2025-05-04 15:30:13</t>
+    <t>2025-05-05 03:14:24</t>
   </si>
   <si>
     <t>2025-05-04 05:36:22</t>
@@ -4141,7 +4141,7 @@
     <t>2025-05-03 21:32:16</t>
   </si>
   <si>
-    <t>2025-05-05 00:31:45</t>
+    <t>2025-05-05 03:44:50</t>
   </si>
   <si>
     <t>2025-05-04 07:23:01</t>
@@ -4327,7 +4327,7 @@
     <t>2025-05-02 18:08:40</t>
   </si>
   <si>
-    <t>2025-05-02 18:00:45</t>
+    <t>2025-05-05 03:44:25</t>
   </si>
   <si>
     <t>2025-05-04 15:03:27</t>
@@ -4660,7 +4660,7 @@
     <t>2025-05-02 07:42:30</t>
   </si>
   <si>
-    <t>2025-05-05 02:13:54</t>
+    <t>2025-05-05 03:21:03</t>
   </si>
   <si>
     <t>2025-05-02 07:29:59</t>
@@ -5203,7 +5203,7 @@
     <t>2025-05-04 12:00:23</t>
   </si>
   <si>
-    <t>2025-05-04 20:23:13</t>
+    <t>2025-05-05 03:40:44</t>
   </si>
   <si>
     <t>2025-05-04 13:15:53</t>
@@ -5272,7 +5272,7 @@
     <t>2025-05-01 06:46:30</t>
   </si>
   <si>
-    <t>2025-05-04 18:20:52</t>
+    <t>2025-05-05 03:46:52</t>
   </si>
   <si>
     <t>2025-04-25 13:50:46</t>
@@ -5431,7 +5431,7 @@
     <t>2025-05-04 18:26:04</t>
   </si>
   <si>
-    <t>2025-05-03 04:54:41</t>
+    <t>2025-05-05 03:45:49</t>
   </si>
   <si>
     <t>2025-05-04 10:15:16</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 07:47:32
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4117,7 +4117,7 @@
     <t>2025-05-04 09:11:06</t>
   </si>
   <si>
-    <t>2025-05-05 03:14:24</t>
+    <t>2025-05-05 04:18:36</t>
   </si>
   <si>
     <t>2025-05-04 05:36:22</t>
@@ -4501,7 +4501,7 @@
     <t>2025-05-02 11:57:16</t>
   </si>
   <si>
-    <t>2025-05-04 06:15:15</t>
+    <t>2025-05-05 04:46:03</t>
   </si>
   <si>
     <t>2025-05-02 11:51:53</t>
@@ -5203,10 +5203,10 @@
     <t>2025-05-04 12:00:23</t>
   </si>
   <si>
-    <t>2025-05-05 03:40:44</t>
-  </si>
-  <si>
-    <t>2025-05-04 13:15:53</t>
+    <t>2025-05-05 04:41:57</t>
+  </si>
+  <si>
+    <t>2025-05-05 04:40:59</t>
   </si>
   <si>
     <t>2025-05-01 08:13:33</t>
@@ -5215,7 +5215,7 @@
     <t>2025-05-04 15:13:24</t>
   </si>
   <si>
-    <t>2025-05-03 16:10:03</t>
+    <t>2025-05-05 04:35:28</t>
   </si>
   <si>
     <t>2025-05-04 17:18:29</t>
@@ -5272,7 +5272,7 @@
     <t>2025-05-01 06:46:30</t>
   </si>
   <si>
-    <t>2025-05-05 03:46:52</t>
+    <t>2025-05-05 04:10:36</t>
   </si>
   <si>
     <t>2025-04-25 13:50:46</t>
@@ -5305,7 +5305,7 @@
     <t>2025-05-04 05:56:39</t>
   </si>
   <si>
-    <t>2025-05-04 08:48:11</t>
+    <t>2025-05-05 04:25:37</t>
   </si>
   <si>
     <t>2025-05-03 16:06:13</t>
@@ -5326,7 +5326,7 @@
     <t>2025-05-04 14:27:10</t>
   </si>
   <si>
-    <t>2025-05-03 16:22:39</t>
+    <t>2025-05-05 04:44:18</t>
   </si>
   <si>
     <t>2025-05-04 06:29:12</t>
@@ -5356,7 +5356,7 @@
     <t>2025-05-02 16:44:34</t>
   </si>
   <si>
-    <t>2025-05-03 11:24:15</t>
+    <t>2025-05-05 04:36:59</t>
   </si>
   <si>
     <t>2025-05-03 12:32:30</t>
@@ -5413,13 +5413,13 @@
     <t>2025-05-04 19:17:08</t>
   </si>
   <si>
-    <t>2025-05-04 17:15:47</t>
+    <t>2025-05-05 04:29:44</t>
   </si>
   <si>
     <t>2025-04-30 13:23:24</t>
   </si>
   <si>
-    <t>2025-05-04 14:11:10</t>
+    <t>2025-05-05 04:34:40</t>
   </si>
   <si>
     <t>2025-05-03 14:36:51</t>
@@ -5443,7 +5443,7 @@
     <t>2025-05-04 21:37:26</t>
   </si>
   <si>
-    <t>2025-05-04 12:09:03</t>
+    <t>2025-05-05 04:37:49</t>
   </si>
   <si>
     <t>2025-05-04 10:22:22</t>
@@ -5467,7 +5467,7 @@
     <t>2025-05-04 10:00:02</t>
   </si>
   <si>
-    <t>2025-05-03 02:47:48</t>
+    <t>2025-05-05 04:43:15</t>
   </si>
   <si>
     <t>2025-04-18 11:04:29</t>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 09:24:22
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4336,7 +4336,7 @@
     <t>2025-05-02 18:08:40</t>
   </si>
   <si>
-    <t>2025-05-05 03:44:25</t>
+    <t>2025-05-05 06:23:05</t>
   </si>
   <si>
     <t>2025-05-04 15:03:27</t>
@@ -4552,7 +4552,7 @@
     <t>2025-05-02 10:32:33</t>
   </si>
   <si>
-    <t>2025-05-02 12:06:36</t>
+    <t>2025-05-05 05:40:46</t>
   </si>
   <si>
     <t>2025-05-03 16:21:03</t>
@@ -4567,7 +4567,7 @@
     <t>2025-05-02 18:21:57</t>
   </si>
   <si>
-    <t>2025-05-02 15:07:22</t>
+    <t>2025-05-05 05:39:38</t>
   </si>
   <si>
     <t>2025-05-02 10:04:41</t>
@@ -4669,7 +4669,7 @@
     <t>2025-05-02 07:42:30</t>
   </si>
   <si>
-    <t>2025-05-05 05:25:48</t>
+    <t>2025-05-05 06:17:45</t>
   </si>
   <si>
     <t>2025-05-02 07:29:59</t>
@@ -5209,10 +5209,10 @@
     <t>2025-05-02 16:39:31</t>
   </si>
   <si>
-    <t>2025-05-05 04:50:11</t>
-  </si>
-  <si>
-    <t>2025-05-05 04:41:57</t>
+    <t>2025-05-05 06:12:37</t>
+  </si>
+  <si>
+    <t>2025-05-05 06:16:20</t>
   </si>
   <si>
     <t>2025-05-05 04:40:59</t>
@@ -5224,7 +5224,7 @@
     <t>2025-05-04 15:13:24</t>
   </si>
   <si>
-    <t>2025-05-05 05:10:27</t>
+    <t>2025-05-05 06:02:27</t>
   </si>
   <si>
     <t>2025-05-04 17:18:29</t>
@@ -5239,7 +5239,7 @@
     <t>2025-05-04 12:40:04</t>
   </si>
   <si>
-    <t>2025-05-05 05:28:11</t>
+    <t>2025-05-05 06:02:20</t>
   </si>
   <si>
     <t>2025-05-01 10:48:58</t>
@@ -5269,7 +5269,7 @@
     <t>2025-04-28 12:44:30</t>
   </si>
   <si>
-    <t>2025-05-02 11:22:41</t>
+    <t>2025-05-05 05:59:02</t>
   </si>
   <si>
     <t>2025-05-04 21:18:15</t>
@@ -5314,13 +5314,13 @@
     <t>2025-05-04 05:56:39</t>
   </si>
   <si>
-    <t>2025-05-05 04:25:37</t>
-  </si>
-  <si>
-    <t>2025-05-03 16:06:13</t>
-  </si>
-  <si>
-    <t>2025-05-01 10:12:55</t>
+    <t>2025-05-05 06:17:44</t>
+  </si>
+  <si>
+    <t>2025-05-05 06:22:35</t>
+  </si>
+  <si>
+    <t>2025-05-05 05:59:24</t>
   </si>
   <si>
     <t>2025-05-02 12:10:06</t>
@@ -5377,7 +5377,7 @@
     <t>2025-05-02 07:30:39</t>
   </si>
   <si>
-    <t>2025-05-03 16:51:22</t>
+    <t>2025-05-05 05:48:06</t>
   </si>
   <si>
     <t>2025-05-04 13:18:13</t>
@@ -5446,7 +5446,7 @@
     <t>2025-05-04 10:15:16</t>
   </si>
   <si>
-    <t>2025-05-05 05:30:00</t>
+    <t>2025-05-05 05:35:01</t>
   </si>
   <si>
     <t>2025-05-04 21:37:26</t>
@@ -5473,7 +5473,7 @@
     <t>2025-04-19 04:32:16</t>
   </si>
   <si>
-    <t>2025-05-04 10:00:02</t>
+    <t>2025-05-05 06:03:45</t>
   </si>
   <si>
     <t>2025-05-05 04:54:55</t>
@@ -19198,7 +19198,7 @@
         <v>0</v>
       </c>
       <c r="H430" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="I430" t="s">
         <v>1300</v>

</xml_diff>

<commit_message>
Update XLSX files - 2025-05-05 10:12:47
</commit_message>
<xml_diff>
--- a/PASSENGERS.xlsx
+++ b/PASSENGERS.xlsx
@@ -4207,7 +4207,7 @@
     <t>2025-05-04 16:30:12</t>
   </si>
   <si>
-    <t>2025-05-04 19:13:50</t>
+    <t>2025-05-05 07:11:20</t>
   </si>
   <si>
     <t>2025-05-04 16:07:45</t>
@@ -4264,7 +4264,7 @@
     <t>2025-05-03 09:57:22</t>
   </si>
   <si>
-    <t>2025-05-03 07:32:31</t>
+    <t>2025-05-05 07:05:15</t>
   </si>
   <si>
     <t>2025-05-03 09:18:46</t>
@@ -4606,7 +4606,7 @@
     <t>2025-05-02 09:47:40</t>
   </si>
   <si>
-    <t>2025-05-04 07:26:38</t>
+    <t>2025-05-05 06:31:02</t>
   </si>
   <si>
     <t>2025-05-02 08:37:20</t>
@@ -4651,10 +4651,10 @@
     <t>2025-05-02 07:57:30</t>
   </si>
   <si>
-    <t>2025-05-02 14:07:58</t>
-  </si>
-  <si>
-    <t>2025-05-03 12:01:59</t>
+    <t>2025-05-05 07:06:31</t>
+  </si>
+  <si>
+    <t>2025-05-05 07:02:37</t>
   </si>
   <si>
     <t>2025-05-04 09:34:23</t>
@@ -4669,7 +4669,7 @@
     <t>2025-05-02 07:42:30</t>
   </si>
   <si>
-    <t>2025-05-05 06:17:45</t>
+    <t>2025-05-05 06:59:52</t>
   </si>
   <si>
     <t>2025-05-02 07:29:59</t>
@@ -4918,7 +4918,7 @@
     <t>2025-05-01 16:39:03</t>
   </si>
   <si>
-    <t>2025-05-01 15:41:29</t>
+    <t>2025-05-05 06:35:15</t>
   </si>
   <si>
     <t>2025-05-01 19:48:30</t>
@@ -5152,7 +5152,7 @@
     <t>2025-05-01 11:00:48</t>
   </si>
   <si>
-    <t>2025-05-03 07:01:50</t>
+    <t>2025-05-05 07:08:14</t>
   </si>
   <si>
     <t>2025-05-03 17:27:35</t>
@@ -5257,7 +5257,7 @@
     <t>2025-05-02 06:18:02</t>
   </si>
   <si>
-    <t>2025-05-05 05:12:45</t>
+    <t>2025-05-05 07:11:05</t>
   </si>
   <si>
     <t>2025-05-01 13:25:35</t>
@@ -5272,7 +5272,7 @@
     <t>2025-05-05 05:59:02</t>
   </si>
   <si>
-    <t>2025-05-04 21:18:15</t>
+    <t>2025-05-05 06:31:23</t>
   </si>
   <si>
     <t>2025-04-30 07:11:42</t>
@@ -5317,7 +5317,7 @@
     <t>2025-05-05 06:17:44</t>
   </si>
   <si>
-    <t>2025-05-05 06:22:35</t>
+    <t>2025-05-05 06:34:03</t>
   </si>
   <si>
     <t>2025-05-05 05:59:24</t>
@@ -5335,7 +5335,7 @@
     <t>2025-05-04 14:27:10</t>
   </si>
   <si>
-    <t>2025-05-05 04:44:18</t>
+    <t>2025-05-05 07:09:50</t>
   </si>
   <si>
     <t>2025-05-04 06:29:12</t>
@@ -5344,7 +5344,7 @@
     <t>2025-05-02 05:21:58</t>
   </si>
   <si>
-    <t>2025-05-05 05:01:26</t>
+    <t>2025-05-05 07:03:08</t>
   </si>
   <si>
     <t>2025-05-02 08:21:28</t>
@@ -5401,16 +5401,16 @@
     <t>2025-05-04 08:28:16</t>
   </si>
   <si>
-    <t>2025-05-04 07:26:52</t>
+    <t>2025-05-05 06:30:09</t>
   </si>
   <si>
     <t>2025-05-02 08:38:09</t>
   </si>
   <si>
-    <t>2025-05-02 12:36:50</t>
-  </si>
-  <si>
-    <t>2025-05-03 17:21:30</t>
+    <t>2025-05-05 07:00:24</t>
+  </si>
+  <si>
+    <t>2025-05-05 07:01:49</t>
   </si>
   <si>
     <t>2025-05-03 11:14:48</t>
@@ -5446,7 +5446,7 @@
     <t>2025-05-04 10:15:16</t>
   </si>
   <si>
-    <t>2025-05-05 05:35:01</t>
+    <t>2025-05-05 07:08:09</t>
   </si>
   <si>
     <t>2025-05-04 21:37:26</t>
@@ -5473,7 +5473,7 @@
     <t>2025-04-19 04:32:16</t>
   </si>
   <si>
-    <t>2025-05-05 06:03:45</t>
+    <t>2025-05-05 06:53:47</t>
   </si>
   <si>
     <t>2025-05-05 04:54:55</t>

</xml_diff>